<commit_message>
Inserimento prime spese pianificate per gennaio 2026
</commit_message>
<xml_diff>
--- a/02-Schede/Calendario_Finanziario_Annuale_2026_v22.xlsx
+++ b/02-Schede/Calendario_Finanziario_Annuale_2026_v22.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1210" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="121">
   <si>
     <t xml:space="preserve">Calendario finanziario mensile</t>
   </si>
@@ -138,6 +138,7 @@
         <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">SDD / Accredito / Bancomat / CC moglie / Contanti / Buoni pasto / Gift card / Altro</t>
     </r>
@@ -302,6 +303,15 @@
     <t xml:space="preserve">CC moglie</t>
   </si>
   <si>
+    <t xml:space="preserve">Utenza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorgenia elettricità</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorgenia gas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abbonamento Disney+ mensile</t>
   </si>
   <si>
@@ -320,9 +330,6 @@
     <t xml:space="preserve">Picco del 15.</t>
   </si>
   <si>
-    <t xml:space="preserve">Utenza</t>
-  </si>
-  <si>
     <t xml:space="preserve">WindTre fibra casa</t>
   </si>
   <si>
@@ -330,15 +337,6 @@
   </si>
   <si>
     <t xml:space="preserve">WindTre figli</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorgenia elettricità (stima)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aggiorna quando arriva la bolletta.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sorgenia gas (stima)</t>
   </si>
   <si>
     <t xml:space="preserve">Auto</t>
@@ -375,6 +373,15 @@
   </si>
   <si>
     <t xml:space="preserve">FEBRUARY 2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorgenia elettricità (stima)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aggiorna quando arriva la bolletta.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sorgenia gas (stima)</t>
   </si>
   <si>
     <t xml:space="preserve">Fisco</t>
@@ -437,7 +444,7 @@
     <numFmt numFmtId="165" formatCode="0.00"/>
     <numFmt numFmtId="166" formatCode="dd/mm"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -479,12 +486,6 @@
       <name val="Cambria"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -677,7 +678,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="7" fillId="3" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -1053,8 +1054,8 @@
   <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="74.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="126.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="126.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="1" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1191,9 +1192,6 @@
       <c r="A30" s="6"/>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B31" s="1"/>
-    </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="5" t="s">
         <v>26</v>
@@ -1202,9 +1200,6 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B33" s="1"/>
-    </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="5" t="s">
         <v>28</v>
@@ -1213,9 +1208,6 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B35" s="1"/>
-    </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="5" t="s">
         <v>30</v>
@@ -1223,9 +1215,6 @@
       <c r="B36" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="1"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="5" t="s">
@@ -1274,7 +1263,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1324,7 +1313,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'06-Jun'!$K$3+$K$2</f>
-        <v>3298.85</v>
+        <v>3285.57</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1429,7 +1418,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -1451,7 +1440,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
@@ -1495,7 +1484,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -1507,7 +1496,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -1519,7 +1508,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -1531,7 +1520,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -1540,10 +1529,10 @@
         <v>46218</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -1555,7 +1544,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -1564,10 +1553,10 @@
         <v>46218</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -1579,7 +1568,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -1588,10 +1577,10 @@
         <v>46218</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -1603,7 +1592,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -1612,10 +1601,10 @@
         <v>46218</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -1627,7 +1616,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -1680,10 +1669,10 @@
         <v>46229</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>-125.56</v>
@@ -1695,7 +1684,7 @@
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -1704,22 +1693,22 @@
         <v>46230</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="G20" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -1728,10 +1717,10 @@
         <v>46234</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -1744,7 +1733,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -1760,7 +1749,7 @@
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -2267,7 +2256,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2317,7 +2306,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'08-Aug'!$K$3+$K$2</f>
-        <v>2743.58</v>
+        <v>2730.3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2422,7 +2411,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -2444,7 +2433,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
@@ -2488,7 +2477,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -2500,7 +2489,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -2512,7 +2501,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -2524,7 +2513,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -2533,10 +2522,10 @@
         <v>46280</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -2548,7 +2537,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -2557,10 +2546,10 @@
         <v>46280</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -2572,7 +2561,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -2581,10 +2570,10 @@
         <v>46280</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -2596,7 +2585,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -2605,10 +2594,10 @@
         <v>46280</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -2620,7 +2609,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -2651,10 +2640,10 @@
         <v>46291</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
@@ -2666,7 +2655,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -2697,22 +2686,22 @@
         <v>46292</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="G20" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -2721,10 +2710,10 @@
         <v>46295</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -2737,7 +2726,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -3258,7 +3247,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3308,7 +3297,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'09-Sep'!$K$3+$K$2</f>
-        <v>2746.04</v>
+        <v>2732.76</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3373,7 +3362,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -3389,7 +3378,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
@@ -3411,7 +3400,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -3455,7 +3444,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -3467,7 +3456,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -3479,7 +3468,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -3491,7 +3480,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -3500,10 +3489,10 @@
         <v>46310</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -3515,7 +3504,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -3524,10 +3513,10 @@
         <v>46310</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -3539,7 +3528,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -3548,10 +3537,10 @@
         <v>46310</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -3563,7 +3552,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -3572,10 +3561,10 @@
         <v>46310</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -3587,7 +3576,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -3640,10 +3629,10 @@
         <v>46321</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
@@ -3655,7 +3644,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -3664,22 +3653,22 @@
         <v>46322</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -3697,7 +3686,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -3710,10 +3699,10 @@
         <v>46326</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -3726,7 +3715,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -4257,7 +4246,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -4307,7 +4296,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'10-Oct'!$K$3+$K$2</f>
-        <v>2188.31</v>
+        <v>2175.03</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4412,7 +4401,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -4434,7 +4423,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
@@ -4478,7 +4467,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -4490,7 +4479,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -4502,7 +4491,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -4514,7 +4503,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -4523,10 +4512,10 @@
         <v>46341</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -4538,7 +4527,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -4547,10 +4536,10 @@
         <v>46341</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -4562,7 +4551,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -4571,10 +4560,10 @@
         <v>46341</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -4586,7 +4575,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -4595,10 +4584,10 @@
         <v>46341</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -4610,7 +4599,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -4641,10 +4630,10 @@
         <v>46352</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
@@ -4656,7 +4645,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -4665,22 +4654,22 @@
         <v>46353</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -4698,7 +4687,7 @@
         <v>-170</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -4711,10 +4700,10 @@
         <v>46356</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>-236.19</v>
@@ -4726,7 +4715,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -4735,10 +4724,10 @@
         <v>46356</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D22" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -4751,7 +4740,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H22" s="18"/>
     </row>
@@ -5262,7 +5251,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -5312,7 +5301,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'11-Nov'!$K$3+$K$2</f>
-        <v>4400.77</v>
+        <v>4387.49</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5393,7 +5382,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
@@ -5415,7 +5404,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -5459,7 +5448,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -5471,7 +5460,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -5483,7 +5472,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -5495,7 +5484,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -5504,10 +5493,10 @@
         <v>46371</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -5519,7 +5508,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -5528,10 +5517,10 @@
         <v>46371</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -5543,7 +5532,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -5552,10 +5541,10 @@
         <v>46371</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -5567,7 +5556,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -5576,10 +5565,10 @@
         <v>46371</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -5591,7 +5580,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -5622,10 +5611,10 @@
         <v>46382</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-125.56</v>
@@ -5637,7 +5626,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -5668,22 +5657,22 @@
         <v>46383</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -5692,20 +5681,20 @@
         <v>46383</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="D20" s="15" t="n">
         <f aca="false">SUMIFS($D:$D,$A:$A,DATE(2026,12,27),$C:$C,"Stipendio netto")</f>
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>95</v>
-      </c>
-      <c r="F20" s="16" t="s">
-        <v>96</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="18"/>
@@ -5715,10 +5704,10 @@
         <v>46387</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -5731,7 +5720,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -6234,7 +6223,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6261,7 +6250,7 @@
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8" t="n">
-        <v>550</v>
+        <v>534.94</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6270,11 +6259,11 @@
       </c>
       <c r="B3" s="8" t="n">
         <f aca="false">'01-Jan'!$K$2</f>
-        <v>308.47</v>
+        <v>295.19</v>
       </c>
       <c r="C3" s="8" t="n">
         <f aca="false">C2+B3</f>
-        <v>858.47</v>
+        <v>830.13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6287,7 +6276,7 @@
       </c>
       <c r="C4" s="8" t="n">
         <f aca="false">C3+B4</f>
-        <v>1134.74</v>
+        <v>1106.4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6300,7 +6289,7 @@
       </c>
       <c r="C5" s="8" t="n">
         <f aca="false">C4+B5</f>
-        <v>1493.2</v>
+        <v>1464.86</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6313,7 +6302,7 @@
       </c>
       <c r="C6" s="8" t="n">
         <f aca="false">C5+B6</f>
-        <v>1665.66</v>
+        <v>1637.32</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6326,7 +6315,7 @@
       </c>
       <c r="C7" s="8" t="n">
         <f aca="false">C6+B7</f>
-        <v>1787.93</v>
+        <v>1759.59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6339,7 +6328,7 @@
       </c>
       <c r="C8" s="8" t="n">
         <f aca="false">C7+B8</f>
-        <v>4170.39</v>
+        <v>4142.05</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6352,7 +6341,7 @@
       </c>
       <c r="C9" s="8" t="n">
         <f aca="false">C8+B9</f>
-        <v>3848.85</v>
+        <v>3820.51</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6365,7 +6354,7 @@
       </c>
       <c r="C10" s="8" t="n">
         <f aca="false">C9+B10</f>
-        <v>3615.12</v>
+        <v>3586.78</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6378,7 +6367,7 @@
       </c>
       <c r="C11" s="8" t="n">
         <f aca="false">C10+B11</f>
-        <v>3293.58</v>
+        <v>3265.24</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6391,7 +6380,7 @@
       </c>
       <c r="C12" s="8" t="n">
         <f aca="false">C11+B12</f>
-        <v>3296.04</v>
+        <v>3267.7</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6404,7 +6393,7 @@
       </c>
       <c r="C13" s="8" t="n">
         <f aca="false">C12+B13</f>
-        <v>2738.31</v>
+        <v>2709.97</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6417,7 +6406,7 @@
       </c>
       <c r="C14" s="8" t="n">
         <f aca="false">C13+B14</f>
-        <v>4950.77</v>
+        <v>4922.43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6426,11 +6415,11 @@
       </c>
       <c r="B15" s="9" t="n">
         <f aca="false">SUM(B3:B14)</f>
-        <v>4400.77</v>
+        <v>4387.49</v>
       </c>
       <c r="C15" s="9" t="n">
         <f aca="false">C14</f>
-        <v>4950.77</v>
+        <v>4922.43</v>
       </c>
     </row>
   </sheetData>
@@ -6454,7 +6443,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6489,7 +6478,7 @@
       </c>
       <c r="K2" s="9" t="n">
         <f aca="false">SUMIF($A:$A,"&lt;&gt;",$D:$D)</f>
-        <v>308.47</v>
+        <v>295.19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6522,7 +6511,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">$K$2</f>
-        <v>308.47</v>
+        <v>295.19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6645,116 +6634,112 @@
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
-        <v>46031</v>
+        <v>46027</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>-6.99</v>
+        <v>-123.71</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
-        <v>46032</v>
+        <v>46027</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>-6.99</v>
+        <v>-29.57</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="n">
-        <v>46032</v>
+        <v>46031</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>0</v>
+        <v>-6.99</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
-        <v>46037</v>
+        <v>46032</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>-218</v>
+        <v>-6.99</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>80</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G12" s="17"/>
       <c r="H12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="13" t="n">
-        <v>46037</v>
+        <v>46032</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>-545</v>
+        <v>0</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>82</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G13" s="17"/>
       <c r="H13" s="18"/>
     </row>
     <row r="14" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6762,22 +6747,22 @@
         <v>46037</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>-31</v>
+        <v>-218</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -6786,19 +6771,19 @@
         <v>46037</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>-14</v>
+        <v>-545</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F15" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G15" s="17" t="s">
         <v>85</v>
@@ -6810,13 +6795,13 @@
         <v>46037</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>-120</v>
+        <v>-31</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>62</v>
@@ -6825,7 +6810,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -6834,13 +6819,13 @@
         <v>46037</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="15" t="n">
-        <v>-20</v>
+        <v>-14</v>
       </c>
       <c r="E17" s="14" t="s">
         <v>62</v>
@@ -6849,7 +6834,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -6902,10 +6887,10 @@
         <v>46048</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>-125.56</v>
@@ -6917,7 +6902,7 @@
         <v>16</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -6926,22 +6911,22 @@
         <v>46049</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E21" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F21" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F21" s="16" t="s">
+      <c r="G21" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G21" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -6959,7 +6944,7 @@
         <v>0</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>18</v>
@@ -6972,10 +6957,10 @@
         <v>46053</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D23" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -7479,7 +7464,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A24" activeCellId="0" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7497,7 +7482,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -7547,7 +7532,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'01-Jan'!$K$3+$K$2</f>
-        <v>584.74</v>
+        <v>571.46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7622,116 +7607,116 @@
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="n">
-        <v>46062</v>
+        <v>46068</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>77</v>
+        <v>101</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>-6.99</v>
+        <v>-120</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="H7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="n">
-        <v>46063</v>
+        <v>46068</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>-6.99</v>
+        <v>-20</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="H8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
-        <v>46067</v>
+        <v>46062</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>0</v>
+        <v>-6.99</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
-        <v>46068</v>
+        <v>46063</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>-218</v>
+        <v>-6.99</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>80</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G10" s="17"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="n">
-        <v>46068</v>
+        <v>46067</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>-545</v>
+        <v>0</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>82</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7739,22 +7724,22 @@
         <v>46068</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>-31</v>
+        <v>-218</v>
       </c>
       <c r="E12" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -7763,19 +7748,19 @@
         <v>46068</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>-14</v>
+        <v>-545</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>85</v>
@@ -7787,13 +7772,13 @@
         <v>46068</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>-120</v>
+        <v>-31</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>62</v>
@@ -7802,7 +7787,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -7811,13 +7796,13 @@
         <v>46068</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>-20</v>
+        <v>-14</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>62</v>
@@ -7826,7 +7811,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -7857,10 +7842,10 @@
         <v>46079</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-125.56</v>
@@ -7872,7 +7857,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -7881,22 +7866,22 @@
         <v>46080</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E18" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="G18" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -7905,10 +7890,10 @@
         <v>46081</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>-236.19</v>
@@ -7920,7 +7905,7 @@
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -7938,7 +7923,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -7951,10 +7936,10 @@
         <v>46081</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -7967,7 +7952,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -8436,27 +8421,27 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F4:F6 F9:F142" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F4:F8 F11:F142" type="list">
       <formula1>"A,B,C,—"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E4:E6 E9:E142" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E4:E8 E11:E142" type="list">
       <formula1>"SDD,Accredito,Bancomat,CC moglie,Contanti,Buoni pasto,Gift card,Altro"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H4:H6 H9:H142" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H4:H8 H11:H142" type="list">
       <formula1>"Sì,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F7:F8" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F9:F10" type="list">
       <formula1>"A,B,C,—"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E7:E8" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E9:E10" type="list">
       <formula1>"SDD,Accredito,Bancomat,CC moglie,Contanti,Buoni pasto,Gift card,Altro"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H7:H8" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H9:H10" type="list">
       <formula1>"Sì,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -8482,7 +8467,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8500,7 +8485,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -8550,7 +8535,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'02-Feb'!$K$3+$K$2</f>
-        <v>943.2</v>
+        <v>929.92</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8627,138 +8612,138 @@
     </row>
     <row r="7" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="13" t="n">
-        <v>46088</v>
+        <v>46096</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="D7" s="15" t="n">
-        <v>0</v>
+        <v>-120</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="17"/>
+      <c r="G7" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="H7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="n">
-        <v>46090</v>
+        <v>46096</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>77</v>
+        <v>103</v>
       </c>
       <c r="D8" s="15" t="n">
-        <v>-6.99</v>
+        <v>-20</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F8" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="17"/>
+        <v>18</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>102</v>
+      </c>
       <c r="H8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="13" t="n">
-        <v>46091</v>
+        <v>46088</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D9" s="15" t="n">
-        <v>-6.99</v>
+        <v>0</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="F9" s="16" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="18"/>
     </row>
     <row r="10" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="13" t="n">
-        <v>46095</v>
+        <v>46090</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="D10" s="15" t="n">
-        <v>0</v>
+        <v>-6.99</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="13" t="n">
-        <v>46096</v>
+        <v>46091</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D11" s="15" t="n">
-        <v>-218</v>
+        <v>-6.99</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>80</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="G11" s="17"/>
       <c r="H11" s="18"/>
     </row>
     <row r="12" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="13" t="n">
-        <v>46096</v>
+        <v>46095</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>60</v>
+        <v>74</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D12" s="15" t="n">
-        <v>-545</v>
+        <v>0</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="F12" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>82</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="G12" s="17"/>
       <c r="H12" s="18"/>
     </row>
     <row r="13" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -8766,22 +8751,22 @@
         <v>46096</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D13" s="15" t="n">
-        <v>-31</v>
+        <v>-218</v>
       </c>
       <c r="E13" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F13" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -8790,19 +8775,19 @@
         <v>46096</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D14" s="15" t="n">
-        <v>-14</v>
+        <v>-545</v>
       </c>
       <c r="E14" s="14" t="s">
         <v>62</v>
       </c>
       <c r="F14" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="G14" s="17" t="s">
         <v>85</v>
@@ -8814,13 +8799,13 @@
         <v>46096</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D15" s="15" t="n">
-        <v>-120</v>
+        <v>-31</v>
       </c>
       <c r="E15" s="14" t="s">
         <v>62</v>
@@ -8829,7 +8814,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -8838,13 +8823,13 @@
         <v>46096</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="15" t="n">
-        <v>-20</v>
+        <v>-14</v>
       </c>
       <c r="E16" s="14" t="s">
         <v>62</v>
@@ -8853,7 +8838,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -8884,10 +8869,10 @@
         <v>46107</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
@@ -8899,7 +8884,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -8908,22 +8893,22 @@
         <v>46108</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -8941,7 +8926,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -8954,10 +8939,10 @@
         <v>46112</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -8970,7 +8955,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -9439,27 +9424,27 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="6">
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F4:F7 F10:F142" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F4:F9 F12:F142" type="list">
       <formula1>"A,B,C,—"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E4:E7 E10:E142" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E4:E9 E12:E142" type="list">
       <formula1>"SDD,Accredito,Bancomat,CC moglie,Contanti,Buoni pasto,Gift card,Altro"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H4:H7 H10:H142" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H4:H9 H12:H142" type="list">
       <formula1>"Sì,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F8:F9" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="F10:F11" type="list">
       <formula1>"A,B,C,—"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E8:E9" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="E10:E11" type="list">
       <formula1>"SDD,Accredito,Bancomat,CC moglie,Contanti,Buoni pasto,Gift card,Altro"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H8:H9" type="list">
+    <dataValidation allowBlank="true" errorStyle="stop" operator="between" showDropDown="false" showErrorMessage="false" showInputMessage="false" sqref="H10:H11" type="list">
       <formula1>"Sì,No"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -9503,7 +9488,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -9553,7 +9538,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'03-Mar'!$K$3+$K$2</f>
-        <v>1115.66</v>
+        <v>1102.38</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -9634,7 +9619,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
@@ -9656,7 +9641,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -9700,7 +9685,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -9712,7 +9697,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -9724,7 +9709,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -9736,7 +9721,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -9745,10 +9730,10 @@
         <v>46127</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -9760,7 +9745,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -9769,10 +9754,10 @@
         <v>46127</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -9784,7 +9769,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -9793,10 +9778,10 @@
         <v>46127</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -9808,7 +9793,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -9817,10 +9802,10 @@
         <v>46127</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -9832,7 +9817,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -9885,10 +9870,10 @@
         <v>46138</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
@@ -9900,7 +9885,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -9909,22 +9894,22 @@
         <v>46139</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -9933,10 +9918,10 @@
         <v>46142</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D20" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -9949,7 +9934,7 @@
         <v>16</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -10480,7 +10465,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -10530,7 +10515,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'04-Apr'!$K$3+$K$2</f>
-        <v>1237.93</v>
+        <v>1224.65</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -10619,7 +10604,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>18</v>
@@ -10657,7 +10642,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
@@ -10679,7 +10664,7 @@
         <v>64</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-6.99</v>
@@ -10701,7 +10686,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -10713,7 +10698,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -10725,7 +10710,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -10737,7 +10722,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -10746,10 +10731,10 @@
         <v>46157</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -10761,7 +10746,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -10770,10 +10755,10 @@
         <v>46157</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -10785,7 +10770,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -10794,10 +10779,10 @@
         <v>46157</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -10809,7 +10794,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -10818,10 +10803,10 @@
         <v>46157</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -10833,7 +10818,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -10886,10 +10871,10 @@
         <v>46168</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>-125.56</v>
@@ -10901,7 +10886,7 @@
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -10910,22 +10895,22 @@
         <v>46169</v>
       </c>
       <c r="B20" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F20" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="G20" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G20" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -10943,7 +10928,7 @@
         <v>0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>18</v>
@@ -10956,10 +10941,10 @@
         <v>46173</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D22" s="15" t="n">
         <v>-236.19</v>
@@ -10971,7 +10956,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H22" s="18"/>
     </row>
@@ -10980,10 +10965,10 @@
         <v>46173</v>
       </c>
       <c r="B23" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D23" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -10996,7 +10981,7 @@
         <v>16</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H23" s="18"/>
     </row>
@@ -11519,7 +11504,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -11569,7 +11554,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'05-May'!$K$3+$K$2</f>
-        <v>3620.39</v>
+        <v>3607.11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11650,7 +11635,7 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
@@ -11672,7 +11657,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -11716,7 +11701,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -11728,7 +11713,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -11740,7 +11725,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -11752,7 +11737,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -11761,10 +11746,10 @@
         <v>46188</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -11776,7 +11761,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -11785,10 +11770,10 @@
         <v>46188</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -11800,7 +11785,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -11809,10 +11794,10 @@
         <v>46188</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -11824,7 +11809,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -11833,10 +11818,10 @@
         <v>46188</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -11848,7 +11833,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -11879,10 +11864,10 @@
         <v>46199</v>
       </c>
       <c r="B17" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C17" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C17" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-125.56</v>
@@ -11894,7 +11879,7 @@
         <v>16</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -11903,22 +11888,22 @@
         <v>46200</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E18" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F18" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="G18" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -11927,23 +11912,23 @@
         <v>46200</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="D19" s="15" t="n">
         <f aca="false">SUMIFS($D:$D,$A:$A,DATE(2026,6,27),$C:$C,"Stipendio netto")</f>
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F19" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="16" t="s">
+      <c r="G19" s="17" t="s">
         <v>96</v>
-      </c>
-      <c r="G19" s="17" t="s">
-        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -11961,7 +11946,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -11974,10 +11959,10 @@
         <v>46203</v>
       </c>
       <c r="B21" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -11990,7 +11975,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -12511,7 +12496,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -12561,7 +12546,7 @@
       </c>
       <c r="K3" s="9" t="n">
         <f aca="false">'07-Jul'!$K$3+$K$2</f>
-        <v>3065.12</v>
+        <v>3051.84</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12626,7 +12611,7 @@
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -12664,7 +12649,7 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
@@ -12686,7 +12671,7 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
@@ -12708,7 +12693,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -12720,7 +12705,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -12732,7 +12717,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -12744,7 +12729,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -12753,10 +12738,10 @@
         <v>46249</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -12768,7 +12753,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -12777,10 +12762,10 @@
         <v>46249</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -12792,7 +12777,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -12801,10 +12786,10 @@
         <v>46249</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -12816,7 +12801,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -12825,10 +12810,10 @@
         <v>46249</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -12840,7 +12825,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -12893,10 +12878,10 @@
         <v>46260</v>
       </c>
       <c r="B18" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
@@ -12906,7 +12891,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -12915,22 +12900,22 @@
         <v>46261</v>
       </c>
       <c r="B19" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="14" t="s">
         <v>93</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -12948,7 +12933,7 @@
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -12961,10 +12946,10 @@
         <v>46265</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>-236.19</v>
@@ -12976,7 +12961,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -12985,10 +12970,10 @@
         <v>46265</v>
       </c>
       <c r="B22" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>99</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>100</v>
       </c>
       <c r="D22" s="15" t="n">
         <f aca="false">-(0)</f>
@@ -13001,7 +12986,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H22" s="18"/>
     </row>

</xml_diff>

<commit_message>
Aggiornamenti del 1° Gennaio
</commit_message>
<xml_diff>
--- a/02-Schede/Calendario_Finanziario_Annuale_2026_v22.xlsx
+++ b/02-Schede/Calendario_Finanziario_Annuale_2026_v22.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1208" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1209" uniqueCount="122">
   <si>
     <t xml:space="preserve">Calendario finanziario mensile</t>
   </si>
@@ -271,6 +271,9 @@
   </si>
   <si>
     <t xml:space="preserve">Spostata al 1°.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sì</t>
   </si>
   <si>
     <t xml:space="preserve">Casa</t>
@@ -1263,7 +1266,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -1369,10 +1372,10 @@
         <v>46204</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-154</v>
@@ -1384,7 +1387,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="18"/>
     </row>
@@ -1393,16 +1396,16 @@
         <v>46207</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>18</v>
@@ -1418,13 +1421,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -1440,13 +1443,13 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>20</v>
@@ -1459,16 +1462,16 @@
         <v>46214</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>18</v>
@@ -1484,7 +1487,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -1496,7 +1499,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -1508,7 +1511,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -1520,7 +1523,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -1529,10 +1532,10 @@
         <v>46218</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -1544,7 +1547,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -1553,10 +1556,10 @@
         <v>46218</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -1568,7 +1571,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -1577,10 +1580,10 @@
         <v>46218</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -1592,7 +1595,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -1601,10 +1604,10 @@
         <v>46218</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -1616,7 +1619,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -1625,16 +1628,16 @@
         <v>46221</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -1647,16 +1650,16 @@
         <v>46228</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>18</v>
@@ -1669,22 +1672,22 @@
         <v>46229</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -1693,22 +1696,22 @@
         <v>46230</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -1717,23 +1720,23 @@
         <v>46234</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -1749,7 +1752,7 @@
     </row>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="21" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -2256,7 +2259,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -2362,10 +2365,10 @@
         <v>46266</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-154</v>
@@ -2377,7 +2380,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="18"/>
     </row>
@@ -2386,16 +2389,16 @@
         <v>46270</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>18</v>
@@ -2411,13 +2414,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -2433,13 +2436,13 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>20</v>
@@ -2452,16 +2455,16 @@
         <v>46277</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>18</v>
@@ -2477,7 +2480,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -2489,7 +2492,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -2501,7 +2504,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -2513,7 +2516,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -2522,10 +2525,10 @@
         <v>46280</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -2537,7 +2540,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -2546,10 +2549,10 @@
         <v>46280</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -2561,7 +2564,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -2570,10 +2573,10 @@
         <v>46280</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -2585,7 +2588,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -2594,10 +2597,10 @@
         <v>46280</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -2609,7 +2612,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -2618,16 +2621,16 @@
         <v>46284</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -2640,22 +2643,22 @@
         <v>46291</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -2664,16 +2667,16 @@
         <v>46291</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>18</v>
@@ -2686,22 +2689,22 @@
         <v>46292</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -2710,23 +2713,23 @@
         <v>46295</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -3247,7 +3250,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -3353,16 +3356,16 @@
         <v>46298</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -3378,13 +3381,13 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>20</v>
@@ -3400,13 +3403,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -3419,16 +3422,16 @@
         <v>46305</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>18</v>
@@ -3444,7 +3447,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -3456,7 +3459,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -3468,7 +3471,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -3480,7 +3483,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -3489,10 +3492,10 @@
         <v>46310</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -3504,7 +3507,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -3513,10 +3516,10 @@
         <v>46310</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -3528,7 +3531,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -3537,10 +3540,10 @@
         <v>46310</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -3552,7 +3555,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -3561,10 +3564,10 @@
         <v>46310</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -3576,7 +3579,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -3585,16 +3588,16 @@
         <v>46312</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>18</v>
@@ -3607,16 +3610,16 @@
         <v>46319</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -3629,22 +3632,22 @@
         <v>46321</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -3653,22 +3656,22 @@
         <v>46322</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -3677,16 +3680,16 @@
         <v>46326</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -3699,23 +3702,23 @@
         <v>46326</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -4246,7 +4249,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -4352,10 +4355,10 @@
         <v>46327</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-154</v>
@@ -4367,7 +4370,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="18"/>
     </row>
@@ -4376,16 +4379,16 @@
         <v>46333</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>18</v>
@@ -4401,13 +4404,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -4423,13 +4426,13 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>20</v>
@@ -4442,16 +4445,16 @@
         <v>46340</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>18</v>
@@ -4467,7 +4470,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -4479,7 +4482,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -4491,7 +4494,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -4503,7 +4506,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -4512,10 +4515,10 @@
         <v>46341</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -4527,7 +4530,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -4536,10 +4539,10 @@
         <v>46341</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -4551,7 +4554,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -4560,10 +4563,10 @@
         <v>46341</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -4575,7 +4578,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -4584,10 +4587,10 @@
         <v>46341</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -4599,7 +4602,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -4608,16 +4611,16 @@
         <v>46347</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -4630,22 +4633,22 @@
         <v>46352</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -4654,22 +4657,22 @@
         <v>46353</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -4678,16 +4681,16 @@
         <v>46354</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -4700,10 +4703,10 @@
         <v>46356</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>-236.19</v>
@@ -4715,7 +4718,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -4724,23 +4727,23 @@
         <v>46356</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D22" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H22" s="18"/>
     </row>
@@ -5251,7 +5254,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -5357,16 +5360,16 @@
         <v>46361</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -5382,13 +5385,13 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>20</v>
@@ -5404,13 +5407,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -5423,16 +5426,16 @@
         <v>46368</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>18</v>
@@ -5448,7 +5451,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -5460,7 +5463,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -5472,7 +5475,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -5484,7 +5487,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -5493,10 +5496,10 @@
         <v>46371</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -5508,7 +5511,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -5517,10 +5520,10 @@
         <v>46371</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -5532,7 +5535,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -5541,10 +5544,10 @@
         <v>46371</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -5556,7 +5559,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -5565,10 +5568,10 @@
         <v>46371</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -5580,7 +5583,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -5589,16 +5592,16 @@
         <v>46375</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>18</v>
@@ -5611,22 +5614,22 @@
         <v>46382</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -5635,16 +5638,16 @@
         <v>46382</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>18</v>
@@ -5657,22 +5660,22 @@
         <v>46383</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -5681,20 +5684,20 @@
         <v>46383</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="D20" s="15" t="n">
         <f aca="false">SUMIFS($D:$D,$A:$A,DATE(2026,12,27),$C:$C,"Stipendio netto")</f>
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G20" s="17"/>
       <c r="H20" s="18"/>
@@ -5704,23 +5707,23 @@
         <v>46387</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -6443,7 +6446,7 @@
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.7578125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6560,17 +6563,19 @@
       <c r="G5" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="18"/>
+      <c r="H5" s="18" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="n">
         <v>46023</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-154</v>
@@ -6582,7 +6587,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="18"/>
     </row>
@@ -6591,22 +6596,22 @@
         <v>46024</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-49.99</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H7" s="18"/>
     </row>
@@ -6615,16 +6620,16 @@
         <v>46025</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>18</v>
@@ -6637,10 +6642,10 @@
         <v>46027</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-123.71</v>
@@ -6659,10 +6664,10 @@
         <v>46027</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-29.57</v>
@@ -6684,13 +6689,13 @@
         <v>64</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>20</v>
@@ -6706,13 +6711,13 @@
         <v>64</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>20</v>
@@ -6725,16 +6730,16 @@
         <v>46032</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F13" s="16" t="s">
         <v>18</v>
@@ -6750,7 +6755,7 @@
         <v>60</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-218</v>
@@ -6762,7 +6767,7 @@
         <v>16</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -6774,7 +6779,7 @@
         <v>60</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-545</v>
@@ -6786,7 +6791,7 @@
         <v>16</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -6795,10 +6800,10 @@
         <v>46037</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-31</v>
@@ -6810,7 +6815,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -6819,10 +6824,10 @@
         <v>46037</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-14</v>
@@ -6834,7 +6839,7 @@
         <v>18</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -6843,16 +6848,16 @@
         <v>46039</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>18</v>
@@ -6865,16 +6870,16 @@
         <v>46046</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>18</v>
@@ -6887,22 +6892,22 @@
         <v>46048</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -6911,22 +6916,22 @@
         <v>46049</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F21" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -6935,16 +6940,16 @@
         <v>46053</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D22" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>18</v>
@@ -6957,17 +6962,17 @@
         <v>46053</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D23" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>16</v>
@@ -7482,7 +7487,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -7588,16 +7593,16 @@
         <v>46060</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -7610,10 +7615,10 @@
         <v>46068</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-120</v>
@@ -7625,7 +7630,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H7" s="18"/>
     </row>
@@ -7634,10 +7639,10 @@
         <v>46068</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-20</v>
@@ -7649,7 +7654,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H8" s="18"/>
     </row>
@@ -7661,13 +7666,13 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>20</v>
@@ -7683,13 +7688,13 @@
         <v>64</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>20</v>
@@ -7702,16 +7707,16 @@
         <v>46067</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>18</v>
@@ -7727,7 +7732,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-218</v>
@@ -7739,7 +7744,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -7751,7 +7756,7 @@
         <v>60</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-545</v>
@@ -7763,7 +7768,7 @@
         <v>16</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -7772,10 +7777,10 @@
         <v>46068</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-31</v>
@@ -7787,7 +7792,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -7796,10 +7801,10 @@
         <v>46068</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-14</v>
@@ -7811,7 +7816,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -7820,16 +7825,16 @@
         <v>46074</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>18</v>
@@ -7842,22 +7847,22 @@
         <v>46079</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -7866,22 +7871,22 @@
         <v>46080</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -7890,10 +7895,10 @@
         <v>46081</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>-236.19</v>
@@ -7905,7 +7910,7 @@
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -7914,16 +7919,16 @@
         <v>46081</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -7936,23 +7941,23 @@
         <v>46081</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -8485,7 +8490,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -8591,10 +8596,10 @@
         <v>46082</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-154</v>
@@ -8606,7 +8611,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="18"/>
     </row>
@@ -8615,10 +8620,10 @@
         <v>46096</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-120</v>
@@ -8630,7 +8635,7 @@
         <v>18</v>
       </c>
       <c r="G7" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H7" s="18"/>
     </row>
@@ -8639,10 +8644,10 @@
         <v>46096</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-20</v>
@@ -8654,7 +8659,7 @@
         <v>18</v>
       </c>
       <c r="G8" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H8" s="18"/>
     </row>
@@ -8663,16 +8668,16 @@
         <v>46088</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>18</v>
@@ -8688,13 +8693,13 @@
         <v>64</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>20</v>
@@ -8710,13 +8715,13 @@
         <v>64</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E11" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F11" s="16" t="s">
         <v>20</v>
@@ -8729,16 +8734,16 @@
         <v>46095</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F12" s="16" t="s">
         <v>18</v>
@@ -8754,7 +8759,7 @@
         <v>60</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-218</v>
@@ -8766,7 +8771,7 @@
         <v>16</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -8778,7 +8783,7 @@
         <v>60</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-545</v>
@@ -8790,7 +8795,7 @@
         <v>16</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -8799,10 +8804,10 @@
         <v>46096</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-31</v>
@@ -8814,7 +8819,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -8823,10 +8828,10 @@
         <v>46096</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-14</v>
@@ -8838,7 +8843,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -8847,16 +8852,16 @@
         <v>46102</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -8869,22 +8874,22 @@
         <v>46107</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -8893,22 +8898,22 @@
         <v>46108</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -8917,16 +8922,16 @@
         <v>46109</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -8939,23 +8944,23 @@
         <v>46112</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -9488,7 +9493,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -9594,16 +9599,16 @@
         <v>46116</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -9619,13 +9624,13 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>20</v>
@@ -9641,13 +9646,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -9660,16 +9665,16 @@
         <v>46123</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>18</v>
@@ -9685,7 +9690,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -9697,7 +9702,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -9709,7 +9714,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -9721,7 +9726,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -9730,10 +9735,10 @@
         <v>46127</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -9745,7 +9750,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -9754,10 +9759,10 @@
         <v>46127</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -9769,7 +9774,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -9778,10 +9783,10 @@
         <v>46127</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -9793,7 +9798,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -9802,10 +9807,10 @@
         <v>46127</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -9817,7 +9822,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -9826,16 +9831,16 @@
         <v>46130</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>18</v>
@@ -9848,16 +9853,16 @@
         <v>46137</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -9870,22 +9875,22 @@
         <v>46138</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -9894,22 +9899,22 @@
         <v>46139</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -9918,23 +9923,23 @@
         <v>46142</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D20" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -10465,7 +10470,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -10571,10 +10576,10 @@
         <v>46143</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-154</v>
@@ -10586,7 +10591,7 @@
         <v>18</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H6" s="18"/>
     </row>
@@ -10595,16 +10600,16 @@
         <v>46144</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>18</v>
@@ -10617,16 +10622,16 @@
         <v>46151</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>18</v>
@@ -10642,13 +10647,13 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>20</v>
@@ -10664,13 +10669,13 @@
         <v>64</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F10" s="16" t="s">
         <v>20</v>
@@ -10686,7 +10691,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-218</v>
@@ -10698,7 +10703,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -10710,7 +10715,7 @@
         <v>60</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-545</v>
@@ -10722,7 +10727,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -10731,10 +10736,10 @@
         <v>46157</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-31</v>
@@ -10746,7 +10751,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -10755,10 +10760,10 @@
         <v>46157</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-14</v>
@@ -10770,7 +10775,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -10779,10 +10784,10 @@
         <v>46157</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-120</v>
@@ -10794,7 +10799,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -10803,10 +10808,10 @@
         <v>46157</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-20</v>
@@ -10818,7 +10823,7 @@
         <v>18</v>
       </c>
       <c r="G16" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H16" s="18"/>
     </row>
@@ -10827,16 +10832,16 @@
         <v>46158</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -10849,16 +10854,16 @@
         <v>46165</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F18" s="16" t="s">
         <v>18</v>
@@ -10871,10 +10876,10 @@
         <v>46168</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>-125.56</v>
@@ -10886,7 +10891,7 @@
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -10895,22 +10900,22 @@
         <v>46169</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F20" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G20" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H20" s="18"/>
     </row>
@@ -10919,16 +10924,16 @@
         <v>46172</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>18</v>
@@ -10941,10 +10946,10 @@
         <v>46173</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D22" s="15" t="n">
         <v>-236.19</v>
@@ -10956,7 +10961,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H22" s="18"/>
     </row>
@@ -10965,23 +10970,23 @@
         <v>46173</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D23" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E23" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G23" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H23" s="18"/>
     </row>
@@ -11504,7 +11509,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -11610,16 +11615,16 @@
         <v>46179</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -11635,13 +11640,13 @@
         <v>64</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>20</v>
@@ -11657,13 +11662,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -11676,16 +11681,16 @@
         <v>46186</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>18</v>
@@ -11701,7 +11706,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -11713,7 +11718,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -11725,7 +11730,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -11737,7 +11742,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -11746,10 +11751,10 @@
         <v>46188</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -11761,7 +11766,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -11770,10 +11775,10 @@
         <v>46188</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -11785,7 +11790,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -11794,10 +11799,10 @@
         <v>46188</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -11809,7 +11814,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -11818,10 +11823,10 @@
         <v>46188</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -11833,7 +11838,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -11842,16 +11847,16 @@
         <v>46193</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>18</v>
@@ -11864,22 +11869,22 @@
         <v>46199</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-125.56</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G17" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H17" s="18"/>
     </row>
@@ -11888,22 +11893,22 @@
         <v>46200</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F18" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -11912,23 +11917,23 @@
         <v>46200</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D19" s="15" t="n">
         <f aca="false">SUMIFS($D:$D,$A:$A,DATE(2026,6,27),$C:$C,"Stipendio netto")</f>
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -11937,16 +11942,16 @@
         <v>46200</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -11959,23 +11964,23 @@
         <v>46203</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D21" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F21" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -12496,7 +12501,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="10" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -12602,16 +12607,16 @@
         <v>46235</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D6" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F6" s="16" t="s">
         <v>18</v>
@@ -12624,16 +12629,16 @@
         <v>46242</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D7" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>18</v>
@@ -12649,13 +12654,13 @@
         <v>64</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D8" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E8" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F8" s="16" t="s">
         <v>20</v>
@@ -12671,13 +12676,13 @@
         <v>64</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D9" s="15" t="n">
         <v>-6.99</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F9" s="16" t="s">
         <v>20</v>
@@ -12693,7 +12698,7 @@
         <v>60</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D10" s="15" t="n">
         <v>-218</v>
@@ -12705,7 +12710,7 @@
         <v>16</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H10" s="18"/>
     </row>
@@ -12717,7 +12722,7 @@
         <v>60</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D11" s="15" t="n">
         <v>-545</v>
@@ -12729,7 +12734,7 @@
         <v>16</v>
       </c>
       <c r="G11" s="17" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H11" s="18"/>
     </row>
@@ -12738,10 +12743,10 @@
         <v>46249</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D12" s="15" t="n">
         <v>-31</v>
@@ -12753,7 +12758,7 @@
         <v>18</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H12" s="18"/>
     </row>
@@ -12762,10 +12767,10 @@
         <v>46249</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D13" s="15" t="n">
         <v>-14</v>
@@ -12777,7 +12782,7 @@
         <v>18</v>
       </c>
       <c r="G13" s="17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H13" s="18"/>
     </row>
@@ -12786,10 +12791,10 @@
         <v>46249</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D14" s="15" t="n">
         <v>-120</v>
@@ -12801,7 +12806,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H14" s="18"/>
     </row>
@@ -12810,10 +12815,10 @@
         <v>46249</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="D15" s="15" t="n">
         <v>-20</v>
@@ -12825,7 +12830,7 @@
         <v>18</v>
       </c>
       <c r="G15" s="17" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H15" s="18"/>
     </row>
@@ -12834,16 +12839,16 @@
         <v>46249</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D16" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F16" s="16" t="s">
         <v>18</v>
@@ -12856,16 +12861,16 @@
         <v>46256</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D17" s="15" t="n">
         <v>-170</v>
       </c>
       <c r="E17" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F17" s="16" t="s">
         <v>18</v>
@@ -12878,10 +12883,10 @@
         <v>46260</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D18" s="15" t="n">
         <v>-125.56</v>
@@ -12891,7 +12896,7 @@
         <v>16</v>
       </c>
       <c r="G18" s="17" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H18" s="18"/>
     </row>
@@ -12900,22 +12905,22 @@
         <v>46261</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="n">
         <v>2380</v>
       </c>
       <c r="E19" s="14" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="F19" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G19" s="17" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H19" s="18"/>
     </row>
@@ -12924,16 +12929,16 @@
         <v>46263</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D20" s="15" t="n">
         <v>0</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>18</v>
@@ -12946,10 +12951,10 @@
         <v>46265</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D21" s="15" t="n">
         <v>-236.19</v>
@@ -12961,7 +12966,7 @@
         <v>16</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H21" s="18"/>
     </row>
@@ -12970,23 +12975,23 @@
         <v>46265</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D22" s="15" t="n">
         <f aca="false">-(0)</f>
         <v>-0</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="F22" s="16" t="s">
         <v>16</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H22" s="18"/>
     </row>

</xml_diff>